<commit_message>
add score columns to recording slips
</commit_message>
<xml_diff>
--- a/howell10.xlsx
+++ b/howell10.xlsx
@@ -536,7 +536,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>For public domain. No rights reserved. Generated on Jan 14, 2026.</t>
+          <t>For public domain. No rights reserved. Generated on Jan 18, 2026.</t>
         </is>
       </c>
     </row>
@@ -711,12 +711,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>PH35</t>
+          <t>PH30</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>PH48</t>
+          <t>PH43</t>
         </is>
       </c>
       <c r="D2" s="4">
@@ -730,12 +730,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>PH58</t>
+          <t>PH82</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>PH79</t>
+          <t>PH90</t>
         </is>
       </c>
       <c r="D3" s="4">
@@ -749,12 +749,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>PH69</t>
+          <t>PH62</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>PH46</t>
+          <t>PH67</t>
         </is>
       </c>
       <c r="D4" s="4">
@@ -768,12 +768,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>PH86</t>
+          <t>PH43</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>PH40</t>
+          <t>PH94</t>
         </is>
       </c>
       <c r="D5" s="4">
@@ -787,12 +787,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>PH80</t>
+          <t>PH68</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>PH23</t>
+          <t>PH68</t>
         </is>
       </c>
       <c r="D6" s="4">
@@ -806,12 +806,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>PH99</t>
+          <t>PH55</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>PH68</t>
+          <t>PH27</t>
         </is>
       </c>
       <c r="D7" s="4">
@@ -825,12 +825,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>PH22</t>
+          <t>PH63</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>PH64</t>
+          <t>PH52</t>
         </is>
       </c>
       <c r="D8" s="4">
@@ -844,12 +844,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>PH96</t>
+          <t>PH55</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>PH75</t>
+          <t>PH43</t>
         </is>
       </c>
       <c r="D9" s="4">
@@ -863,12 +863,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>PH24</t>
+          <t>PH86</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>PH34</t>
+          <t>PH75</t>
         </is>
       </c>
       <c r="D10" s="4">
@@ -882,12 +882,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>PH23</t>
+          <t>PH44</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>PH87</t>
+          <t>PH51</t>
         </is>
       </c>
       <c r="D11" s="4">
@@ -1516,23 +1516,23 @@
         </is>
       </c>
       <c r="G8">
-        <f>'By Round'!G3</f>
+        <f>'By Round'!G2</f>
         <v/>
       </c>
       <c r="H8">
-        <f>'By Round'!H3</f>
+        <f>'By Round'!H2</f>
         <v/>
       </c>
       <c r="I8">
-        <f>'By Round'!I3</f>
+        <f>'By Round'!I2</f>
         <v/>
       </c>
       <c r="J8">
-        <f>'By Round'!J3</f>
+        <f>'By Round'!J2</f>
         <v/>
       </c>
       <c r="K8">
-        <f>'By Round'!K3</f>
+        <f>'By Round'!K2</f>
         <v/>
       </c>
       <c r="L8" s="11">
@@ -1607,23 +1607,23 @@
         </is>
       </c>
       <c r="G9">
-        <f>'By Round'!G21</f>
+        <f>'By Round'!G20</f>
         <v/>
       </c>
       <c r="H9">
-        <f>'By Round'!H21</f>
+        <f>'By Round'!H20</f>
         <v/>
       </c>
       <c r="I9">
-        <f>'By Round'!I21</f>
+        <f>'By Round'!I20</f>
         <v/>
       </c>
       <c r="J9">
-        <f>'By Round'!J21</f>
+        <f>'By Round'!J20</f>
         <v/>
       </c>
       <c r="K9">
-        <f>'By Round'!K21</f>
+        <f>'By Round'!K20</f>
         <v/>
       </c>
       <c r="L9" s="11">
@@ -1698,23 +1698,23 @@
         </is>
       </c>
       <c r="G10">
-        <f>'By Round'!G29</f>
+        <f>'By Round'!G28</f>
         <v/>
       </c>
       <c r="H10">
-        <f>'By Round'!H29</f>
+        <f>'By Round'!H28</f>
         <v/>
       </c>
       <c r="I10">
-        <f>'By Round'!I29</f>
+        <f>'By Round'!I28</f>
         <v/>
       </c>
       <c r="J10">
-        <f>'By Round'!J29</f>
+        <f>'By Round'!J28</f>
         <v/>
       </c>
       <c r="K10">
-        <f>'By Round'!K29</f>
+        <f>'By Round'!K28</f>
         <v/>
       </c>
       <c r="L10" s="11">
@@ -1789,23 +1789,23 @@
         </is>
       </c>
       <c r="G11">
-        <f>'By Round'!G77</f>
+        <f>'By Round'!G76</f>
         <v/>
       </c>
       <c r="H11">
-        <f>'By Round'!H77</f>
+        <f>'By Round'!H76</f>
         <v/>
       </c>
       <c r="I11">
-        <f>'By Round'!I77</f>
+        <f>'By Round'!I76</f>
         <v/>
       </c>
       <c r="J11">
-        <f>'By Round'!J77</f>
+        <f>'By Round'!J76</f>
         <v/>
       </c>
       <c r="K11">
-        <f>'By Round'!K77</f>
+        <f>'By Round'!K76</f>
         <v/>
       </c>
       <c r="L11" s="11">
@@ -1880,23 +1880,23 @@
         </is>
       </c>
       <c r="G12">
-        <f>'By Round'!G85</f>
+        <f>'By Round'!G84</f>
         <v/>
       </c>
       <c r="H12">
-        <f>'By Round'!H85</f>
+        <f>'By Round'!H84</f>
         <v/>
       </c>
       <c r="I12">
-        <f>'By Round'!I85</f>
+        <f>'By Round'!I84</f>
         <v/>
       </c>
       <c r="J12">
-        <f>'By Round'!J85</f>
+        <f>'By Round'!J84</f>
         <v/>
       </c>
       <c r="K12">
-        <f>'By Round'!K85</f>
+        <f>'By Round'!K84</f>
         <v/>
       </c>
       <c r="L12" s="11">
@@ -2432,23 +2432,23 @@
         </is>
       </c>
       <c r="G18">
-        <f>'By Round'!G5</f>
+        <f>'By Round'!G4</f>
         <v/>
       </c>
       <c r="H18">
-        <f>'By Round'!H5</f>
+        <f>'By Round'!H4</f>
         <v/>
       </c>
       <c r="I18">
-        <f>'By Round'!I5</f>
+        <f>'By Round'!I4</f>
         <v/>
       </c>
       <c r="J18">
-        <f>'By Round'!J5</f>
+        <f>'By Round'!J4</f>
         <v/>
       </c>
       <c r="K18">
-        <f>'By Round'!K5</f>
+        <f>'By Round'!K4</f>
         <v/>
       </c>
       <c r="L18" s="11">
@@ -2523,23 +2523,23 @@
         </is>
       </c>
       <c r="G19">
-        <f>'By Round'!G13</f>
+        <f>'By Round'!G12</f>
         <v/>
       </c>
       <c r="H19">
-        <f>'By Round'!H13</f>
+        <f>'By Round'!H12</f>
         <v/>
       </c>
       <c r="I19">
-        <f>'By Round'!I13</f>
+        <f>'By Round'!I12</f>
         <v/>
       </c>
       <c r="J19">
-        <f>'By Round'!J13</f>
+        <f>'By Round'!J12</f>
         <v/>
       </c>
       <c r="K19">
-        <f>'By Round'!K13</f>
+        <f>'By Round'!K12</f>
         <v/>
       </c>
       <c r="L19" s="11">
@@ -2614,23 +2614,23 @@
         </is>
       </c>
       <c r="G20">
-        <f>'By Round'!G31</f>
+        <f>'By Round'!G30</f>
         <v/>
       </c>
       <c r="H20">
-        <f>'By Round'!H31</f>
+        <f>'By Round'!H30</f>
         <v/>
       </c>
       <c r="I20">
-        <f>'By Round'!I31</f>
+        <f>'By Round'!I30</f>
         <v/>
       </c>
       <c r="J20">
-        <f>'By Round'!J31</f>
+        <f>'By Round'!J30</f>
         <v/>
       </c>
       <c r="K20">
-        <f>'By Round'!K31</f>
+        <f>'By Round'!K30</f>
         <v/>
       </c>
       <c r="L20" s="11">
@@ -2705,23 +2705,23 @@
         </is>
       </c>
       <c r="G21">
-        <f>'By Round'!G39</f>
+        <f>'By Round'!G38</f>
         <v/>
       </c>
       <c r="H21">
-        <f>'By Round'!H39</f>
+        <f>'By Round'!H38</f>
         <v/>
       </c>
       <c r="I21">
-        <f>'By Round'!I39</f>
+        <f>'By Round'!I38</f>
         <v/>
       </c>
       <c r="J21">
-        <f>'By Round'!J39</f>
+        <f>'By Round'!J38</f>
         <v/>
       </c>
       <c r="K21">
-        <f>'By Round'!K39</f>
+        <f>'By Round'!K38</f>
         <v/>
       </c>
       <c r="L21" s="11">
@@ -2796,23 +2796,23 @@
         </is>
       </c>
       <c r="G22">
-        <f>'By Round'!G87</f>
+        <f>'By Round'!G86</f>
         <v/>
       </c>
       <c r="H22">
-        <f>'By Round'!H87</f>
+        <f>'By Round'!H86</f>
         <v/>
       </c>
       <c r="I22">
-        <f>'By Round'!I87</f>
+        <f>'By Round'!I86</f>
         <v/>
       </c>
       <c r="J22">
-        <f>'By Round'!J87</f>
+        <f>'By Round'!J86</f>
         <v/>
       </c>
       <c r="K22">
-        <f>'By Round'!K87</f>
+        <f>'By Round'!K86</f>
         <v/>
       </c>
       <c r="L22" s="11">
@@ -3348,23 +3348,23 @@
         </is>
       </c>
       <c r="G28">
-        <f>'By Round'!G7</f>
+        <f>'By Round'!G6</f>
         <v/>
       </c>
       <c r="H28">
-        <f>'By Round'!H7</f>
+        <f>'By Round'!H6</f>
         <v/>
       </c>
       <c r="I28">
-        <f>'By Round'!I7</f>
+        <f>'By Round'!I6</f>
         <v/>
       </c>
       <c r="J28">
-        <f>'By Round'!J7</f>
+        <f>'By Round'!J6</f>
         <v/>
       </c>
       <c r="K28">
-        <f>'By Round'!K7</f>
+        <f>'By Round'!K6</f>
         <v/>
       </c>
       <c r="L28" s="11">
@@ -3439,23 +3439,23 @@
         </is>
       </c>
       <c r="G29">
-        <f>'By Round'!G15</f>
+        <f>'By Round'!G14</f>
         <v/>
       </c>
       <c r="H29">
-        <f>'By Round'!H15</f>
+        <f>'By Round'!H14</f>
         <v/>
       </c>
       <c r="I29">
-        <f>'By Round'!I15</f>
+        <f>'By Round'!I14</f>
         <v/>
       </c>
       <c r="J29">
-        <f>'By Round'!J15</f>
+        <f>'By Round'!J14</f>
         <v/>
       </c>
       <c r="K29">
-        <f>'By Round'!K15</f>
+        <f>'By Round'!K14</f>
         <v/>
       </c>
       <c r="L29" s="11">
@@ -3530,23 +3530,23 @@
         </is>
       </c>
       <c r="G30">
-        <f>'By Round'!G23</f>
+        <f>'By Round'!G22</f>
         <v/>
       </c>
       <c r="H30">
-        <f>'By Round'!H23</f>
+        <f>'By Round'!H22</f>
         <v/>
       </c>
       <c r="I30">
-        <f>'By Round'!I23</f>
+        <f>'By Round'!I22</f>
         <v/>
       </c>
       <c r="J30">
-        <f>'By Round'!J23</f>
+        <f>'By Round'!J22</f>
         <v/>
       </c>
       <c r="K30">
-        <f>'By Round'!K23</f>
+        <f>'By Round'!K22</f>
         <v/>
       </c>
       <c r="L30" s="11">
@@ -3621,23 +3621,23 @@
         </is>
       </c>
       <c r="G31">
-        <f>'By Round'!G41</f>
+        <f>'By Round'!G40</f>
         <v/>
       </c>
       <c r="H31">
-        <f>'By Round'!H41</f>
+        <f>'By Round'!H40</f>
         <v/>
       </c>
       <c r="I31">
-        <f>'By Round'!I41</f>
+        <f>'By Round'!I40</f>
         <v/>
       </c>
       <c r="J31">
-        <f>'By Round'!J41</f>
+        <f>'By Round'!J40</f>
         <v/>
       </c>
       <c r="K31">
-        <f>'By Round'!K41</f>
+        <f>'By Round'!K40</f>
         <v/>
       </c>
       <c r="L31" s="11">
@@ -3712,23 +3712,23 @@
         </is>
       </c>
       <c r="G32">
-        <f>'By Round'!G49</f>
+        <f>'By Round'!G48</f>
         <v/>
       </c>
       <c r="H32">
-        <f>'By Round'!H49</f>
+        <f>'By Round'!H48</f>
         <v/>
       </c>
       <c r="I32">
-        <f>'By Round'!I49</f>
+        <f>'By Round'!I48</f>
         <v/>
       </c>
       <c r="J32">
-        <f>'By Round'!J49</f>
+        <f>'By Round'!J48</f>
         <v/>
       </c>
       <c r="K32">
-        <f>'By Round'!K49</f>
+        <f>'By Round'!K48</f>
         <v/>
       </c>
       <c r="L32" s="11">
@@ -4264,23 +4264,23 @@
         </is>
       </c>
       <c r="G38">
-        <f>'By Round'!G17</f>
+        <f>'By Round'!G16</f>
         <v/>
       </c>
       <c r="H38">
-        <f>'By Round'!H17</f>
+        <f>'By Round'!H16</f>
         <v/>
       </c>
       <c r="I38">
-        <f>'By Round'!I17</f>
+        <f>'By Round'!I16</f>
         <v/>
       </c>
       <c r="J38">
-        <f>'By Round'!J17</f>
+        <f>'By Round'!J16</f>
         <v/>
       </c>
       <c r="K38">
-        <f>'By Round'!K17</f>
+        <f>'By Round'!K16</f>
         <v/>
       </c>
       <c r="L38" s="11">
@@ -4355,23 +4355,23 @@
         </is>
       </c>
       <c r="G39">
-        <f>'By Round'!G25</f>
+        <f>'By Round'!G24</f>
         <v/>
       </c>
       <c r="H39">
-        <f>'By Round'!H25</f>
+        <f>'By Round'!H24</f>
         <v/>
       </c>
       <c r="I39">
-        <f>'By Round'!I25</f>
+        <f>'By Round'!I24</f>
         <v/>
       </c>
       <c r="J39">
-        <f>'By Round'!J25</f>
+        <f>'By Round'!J24</f>
         <v/>
       </c>
       <c r="K39">
-        <f>'By Round'!K25</f>
+        <f>'By Round'!K24</f>
         <v/>
       </c>
       <c r="L39" s="11">
@@ -4446,23 +4446,23 @@
         </is>
       </c>
       <c r="G40">
-        <f>'By Round'!G33</f>
+        <f>'By Round'!G32</f>
         <v/>
       </c>
       <c r="H40">
-        <f>'By Round'!H33</f>
+        <f>'By Round'!H32</f>
         <v/>
       </c>
       <c r="I40">
-        <f>'By Round'!I33</f>
+        <f>'By Round'!I32</f>
         <v/>
       </c>
       <c r="J40">
-        <f>'By Round'!J33</f>
+        <f>'By Round'!J32</f>
         <v/>
       </c>
       <c r="K40">
-        <f>'By Round'!K33</f>
+        <f>'By Round'!K32</f>
         <v/>
       </c>
       <c r="L40" s="11">
@@ -4537,23 +4537,23 @@
         </is>
       </c>
       <c r="G41">
-        <f>'By Round'!G51</f>
+        <f>'By Round'!G50</f>
         <v/>
       </c>
       <c r="H41">
-        <f>'By Round'!H51</f>
+        <f>'By Round'!H50</f>
         <v/>
       </c>
       <c r="I41">
-        <f>'By Round'!I51</f>
+        <f>'By Round'!I50</f>
         <v/>
       </c>
       <c r="J41">
-        <f>'By Round'!J51</f>
+        <f>'By Round'!J50</f>
         <v/>
       </c>
       <c r="K41">
-        <f>'By Round'!K51</f>
+        <f>'By Round'!K50</f>
         <v/>
       </c>
       <c r="L41" s="11">
@@ -4628,23 +4628,23 @@
         </is>
       </c>
       <c r="G42">
-        <f>'By Round'!G59</f>
+        <f>'By Round'!G58</f>
         <v/>
       </c>
       <c r="H42">
-        <f>'By Round'!H59</f>
+        <f>'By Round'!H58</f>
         <v/>
       </c>
       <c r="I42">
-        <f>'By Round'!I59</f>
+        <f>'By Round'!I58</f>
         <v/>
       </c>
       <c r="J42">
-        <f>'By Round'!J59</f>
+        <f>'By Round'!J58</f>
         <v/>
       </c>
       <c r="K42">
-        <f>'By Round'!K59</f>
+        <f>'By Round'!K58</f>
         <v/>
       </c>
       <c r="L42" s="11">
@@ -5180,23 +5180,23 @@
         </is>
       </c>
       <c r="G48">
-        <f>'By Round'!G27</f>
+        <f>'By Round'!G26</f>
         <v/>
       </c>
       <c r="H48">
-        <f>'By Round'!H27</f>
+        <f>'By Round'!H26</f>
         <v/>
       </c>
       <c r="I48">
-        <f>'By Round'!I27</f>
+        <f>'By Round'!I26</f>
         <v/>
       </c>
       <c r="J48">
-        <f>'By Round'!J27</f>
+        <f>'By Round'!J26</f>
         <v/>
       </c>
       <c r="K48">
-        <f>'By Round'!K27</f>
+        <f>'By Round'!K26</f>
         <v/>
       </c>
       <c r="L48" s="11">
@@ -5271,23 +5271,23 @@
         </is>
       </c>
       <c r="G49">
-        <f>'By Round'!G35</f>
+        <f>'By Round'!G34</f>
         <v/>
       </c>
       <c r="H49">
-        <f>'By Round'!H35</f>
+        <f>'By Round'!H34</f>
         <v/>
       </c>
       <c r="I49">
-        <f>'By Round'!I35</f>
+        <f>'By Round'!I34</f>
         <v/>
       </c>
       <c r="J49">
-        <f>'By Round'!J35</f>
+        <f>'By Round'!J34</f>
         <v/>
       </c>
       <c r="K49">
-        <f>'By Round'!K35</f>
+        <f>'By Round'!K34</f>
         <v/>
       </c>
       <c r="L49" s="11">
@@ -5362,23 +5362,23 @@
         </is>
       </c>
       <c r="G50">
-        <f>'By Round'!G43</f>
+        <f>'By Round'!G42</f>
         <v/>
       </c>
       <c r="H50">
-        <f>'By Round'!H43</f>
+        <f>'By Round'!H42</f>
         <v/>
       </c>
       <c r="I50">
-        <f>'By Round'!I43</f>
+        <f>'By Round'!I42</f>
         <v/>
       </c>
       <c r="J50">
-        <f>'By Round'!J43</f>
+        <f>'By Round'!J42</f>
         <v/>
       </c>
       <c r="K50">
-        <f>'By Round'!K43</f>
+        <f>'By Round'!K42</f>
         <v/>
       </c>
       <c r="L50" s="11">
@@ -5453,23 +5453,23 @@
         </is>
       </c>
       <c r="G51">
-        <f>'By Round'!G61</f>
+        <f>'By Round'!G60</f>
         <v/>
       </c>
       <c r="H51">
-        <f>'By Round'!H61</f>
+        <f>'By Round'!H60</f>
         <v/>
       </c>
       <c r="I51">
-        <f>'By Round'!I61</f>
+        <f>'By Round'!I60</f>
         <v/>
       </c>
       <c r="J51">
-        <f>'By Round'!J61</f>
+        <f>'By Round'!J60</f>
         <v/>
       </c>
       <c r="K51">
-        <f>'By Round'!K61</f>
+        <f>'By Round'!K60</f>
         <v/>
       </c>
       <c r="L51" s="11">
@@ -5544,23 +5544,23 @@
         </is>
       </c>
       <c r="G52">
-        <f>'By Round'!G69</f>
+        <f>'By Round'!G68</f>
         <v/>
       </c>
       <c r="H52">
-        <f>'By Round'!H69</f>
+        <f>'By Round'!H68</f>
         <v/>
       </c>
       <c r="I52">
-        <f>'By Round'!I69</f>
+        <f>'By Round'!I68</f>
         <v/>
       </c>
       <c r="J52">
-        <f>'By Round'!J69</f>
+        <f>'By Round'!J68</f>
         <v/>
       </c>
       <c r="K52">
-        <f>'By Round'!K69</f>
+        <f>'By Round'!K68</f>
         <v/>
       </c>
       <c r="L52" s="11">
@@ -6096,23 +6096,23 @@
         </is>
       </c>
       <c r="G58">
-        <f>'By Round'!G37</f>
+        <f>'By Round'!G36</f>
         <v/>
       </c>
       <c r="H58">
-        <f>'By Round'!H37</f>
+        <f>'By Round'!H36</f>
         <v/>
       </c>
       <c r="I58">
-        <f>'By Round'!I37</f>
+        <f>'By Round'!I36</f>
         <v/>
       </c>
       <c r="J58">
-        <f>'By Round'!J37</f>
+        <f>'By Round'!J36</f>
         <v/>
       </c>
       <c r="K58">
-        <f>'By Round'!K37</f>
+        <f>'By Round'!K36</f>
         <v/>
       </c>
       <c r="L58" s="11">
@@ -6187,23 +6187,23 @@
         </is>
       </c>
       <c r="G59">
-        <f>'By Round'!G45</f>
+        <f>'By Round'!G44</f>
         <v/>
       </c>
       <c r="H59">
-        <f>'By Round'!H45</f>
+        <f>'By Round'!H44</f>
         <v/>
       </c>
       <c r="I59">
-        <f>'By Round'!I45</f>
+        <f>'By Round'!I44</f>
         <v/>
       </c>
       <c r="J59">
-        <f>'By Round'!J45</f>
+        <f>'By Round'!J44</f>
         <v/>
       </c>
       <c r="K59">
-        <f>'By Round'!K45</f>
+        <f>'By Round'!K44</f>
         <v/>
       </c>
       <c r="L59" s="11">
@@ -6278,23 +6278,23 @@
         </is>
       </c>
       <c r="G60">
-        <f>'By Round'!G53</f>
+        <f>'By Round'!G52</f>
         <v/>
       </c>
       <c r="H60">
-        <f>'By Round'!H53</f>
+        <f>'By Round'!H52</f>
         <v/>
       </c>
       <c r="I60">
-        <f>'By Round'!I53</f>
+        <f>'By Round'!I52</f>
         <v/>
       </c>
       <c r="J60">
-        <f>'By Round'!J53</f>
+        <f>'By Round'!J52</f>
         <v/>
       </c>
       <c r="K60">
-        <f>'By Round'!K53</f>
+        <f>'By Round'!K52</f>
         <v/>
       </c>
       <c r="L60" s="11">
@@ -6369,23 +6369,23 @@
         </is>
       </c>
       <c r="G61">
-        <f>'By Round'!G71</f>
+        <f>'By Round'!G70</f>
         <v/>
       </c>
       <c r="H61">
-        <f>'By Round'!H71</f>
+        <f>'By Round'!H70</f>
         <v/>
       </c>
       <c r="I61">
-        <f>'By Round'!I71</f>
+        <f>'By Round'!I70</f>
         <v/>
       </c>
       <c r="J61">
-        <f>'By Round'!J71</f>
+        <f>'By Round'!J70</f>
         <v/>
       </c>
       <c r="K61">
-        <f>'By Round'!K71</f>
+        <f>'By Round'!K70</f>
         <v/>
       </c>
       <c r="L61" s="11">
@@ -6460,23 +6460,23 @@
         </is>
       </c>
       <c r="G62">
-        <f>'By Round'!G79</f>
+        <f>'By Round'!G78</f>
         <v/>
       </c>
       <c r="H62">
-        <f>'By Round'!H79</f>
+        <f>'By Round'!H78</f>
         <v/>
       </c>
       <c r="I62">
-        <f>'By Round'!I79</f>
+        <f>'By Round'!I78</f>
         <v/>
       </c>
       <c r="J62">
-        <f>'By Round'!J79</f>
+        <f>'By Round'!J78</f>
         <v/>
       </c>
       <c r="K62">
-        <f>'By Round'!K79</f>
+        <f>'By Round'!K78</f>
         <v/>
       </c>
       <c r="L62" s="11">
@@ -7012,23 +7012,23 @@
         </is>
       </c>
       <c r="G68">
-        <f>'By Round'!G47</f>
+        <f>'By Round'!G46</f>
         <v/>
       </c>
       <c r="H68">
-        <f>'By Round'!H47</f>
+        <f>'By Round'!H46</f>
         <v/>
       </c>
       <c r="I68">
-        <f>'By Round'!I47</f>
+        <f>'By Round'!I46</f>
         <v/>
       </c>
       <c r="J68">
-        <f>'By Round'!J47</f>
+        <f>'By Round'!J46</f>
         <v/>
       </c>
       <c r="K68">
-        <f>'By Round'!K47</f>
+        <f>'By Round'!K46</f>
         <v/>
       </c>
       <c r="L68" s="11">
@@ -7103,23 +7103,23 @@
         </is>
       </c>
       <c r="G69">
-        <f>'By Round'!G55</f>
+        <f>'By Round'!G54</f>
         <v/>
       </c>
       <c r="H69">
-        <f>'By Round'!H55</f>
+        <f>'By Round'!H54</f>
         <v/>
       </c>
       <c r="I69">
-        <f>'By Round'!I55</f>
+        <f>'By Round'!I54</f>
         <v/>
       </c>
       <c r="J69">
-        <f>'By Round'!J55</f>
+        <f>'By Round'!J54</f>
         <v/>
       </c>
       <c r="K69">
-        <f>'By Round'!K55</f>
+        <f>'By Round'!K54</f>
         <v/>
       </c>
       <c r="L69" s="11">
@@ -7194,23 +7194,23 @@
         </is>
       </c>
       <c r="G70">
-        <f>'By Round'!G63</f>
+        <f>'By Round'!G62</f>
         <v/>
       </c>
       <c r="H70">
-        <f>'By Round'!H63</f>
+        <f>'By Round'!H62</f>
         <v/>
       </c>
       <c r="I70">
-        <f>'By Round'!I63</f>
+        <f>'By Round'!I62</f>
         <v/>
       </c>
       <c r="J70">
-        <f>'By Round'!J63</f>
+        <f>'By Round'!J62</f>
         <v/>
       </c>
       <c r="K70">
-        <f>'By Round'!K63</f>
+        <f>'By Round'!K62</f>
         <v/>
       </c>
       <c r="L70" s="11">
@@ -7285,23 +7285,23 @@
         </is>
       </c>
       <c r="G71">
-        <f>'By Round'!G81</f>
+        <f>'By Round'!G80</f>
         <v/>
       </c>
       <c r="H71">
-        <f>'By Round'!H81</f>
+        <f>'By Round'!H80</f>
         <v/>
       </c>
       <c r="I71">
-        <f>'By Round'!I81</f>
+        <f>'By Round'!I80</f>
         <v/>
       </c>
       <c r="J71">
-        <f>'By Round'!J81</f>
+        <f>'By Round'!J80</f>
         <v/>
       </c>
       <c r="K71">
-        <f>'By Round'!K81</f>
+        <f>'By Round'!K80</f>
         <v/>
       </c>
       <c r="L71" s="11">
@@ -7376,23 +7376,23 @@
         </is>
       </c>
       <c r="G72">
-        <f>'By Round'!G89</f>
+        <f>'By Round'!G88</f>
         <v/>
       </c>
       <c r="H72">
-        <f>'By Round'!H89</f>
+        <f>'By Round'!H88</f>
         <v/>
       </c>
       <c r="I72">
-        <f>'By Round'!I89</f>
+        <f>'By Round'!I88</f>
         <v/>
       </c>
       <c r="J72">
-        <f>'By Round'!J89</f>
+        <f>'By Round'!J88</f>
         <v/>
       </c>
       <c r="K72">
-        <f>'By Round'!K89</f>
+        <f>'By Round'!K88</f>
         <v/>
       </c>
       <c r="L72" s="11">
@@ -7928,23 +7928,23 @@
         </is>
       </c>
       <c r="G78">
-        <f>'By Round'!G9</f>
+        <f>'By Round'!G8</f>
         <v/>
       </c>
       <c r="H78">
-        <f>'By Round'!H9</f>
+        <f>'By Round'!H8</f>
         <v/>
       </c>
       <c r="I78">
-        <f>'By Round'!I9</f>
+        <f>'By Round'!I8</f>
         <v/>
       </c>
       <c r="J78">
-        <f>'By Round'!J9</f>
+        <f>'By Round'!J8</f>
         <v/>
       </c>
       <c r="K78">
-        <f>'By Round'!K9</f>
+        <f>'By Round'!K8</f>
         <v/>
       </c>
       <c r="L78" s="11">
@@ -8019,23 +8019,23 @@
         </is>
       </c>
       <c r="G79">
-        <f>'By Round'!G57</f>
+        <f>'By Round'!G56</f>
         <v/>
       </c>
       <c r="H79">
-        <f>'By Round'!H57</f>
+        <f>'By Round'!H56</f>
         <v/>
       </c>
       <c r="I79">
-        <f>'By Round'!I57</f>
+        <f>'By Round'!I56</f>
         <v/>
       </c>
       <c r="J79">
-        <f>'By Round'!J57</f>
+        <f>'By Round'!J56</f>
         <v/>
       </c>
       <c r="K79">
-        <f>'By Round'!K57</f>
+        <f>'By Round'!K56</f>
         <v/>
       </c>
       <c r="L79" s="11">
@@ -8110,23 +8110,23 @@
         </is>
       </c>
       <c r="G80">
-        <f>'By Round'!G65</f>
+        <f>'By Round'!G64</f>
         <v/>
       </c>
       <c r="H80">
-        <f>'By Round'!H65</f>
+        <f>'By Round'!H64</f>
         <v/>
       </c>
       <c r="I80">
-        <f>'By Round'!I65</f>
+        <f>'By Round'!I64</f>
         <v/>
       </c>
       <c r="J80">
-        <f>'By Round'!J65</f>
+        <f>'By Round'!J64</f>
         <v/>
       </c>
       <c r="K80">
-        <f>'By Round'!K65</f>
+        <f>'By Round'!K64</f>
         <v/>
       </c>
       <c r="L80" s="11">
@@ -8201,23 +8201,23 @@
         </is>
       </c>
       <c r="G81">
-        <f>'By Round'!G73</f>
+        <f>'By Round'!G72</f>
         <v/>
       </c>
       <c r="H81">
-        <f>'By Round'!H73</f>
+        <f>'By Round'!H72</f>
         <v/>
       </c>
       <c r="I81">
-        <f>'By Round'!I73</f>
+        <f>'By Round'!I72</f>
         <v/>
       </c>
       <c r="J81">
-        <f>'By Round'!J73</f>
+        <f>'By Round'!J72</f>
         <v/>
       </c>
       <c r="K81">
-        <f>'By Round'!K73</f>
+        <f>'By Round'!K72</f>
         <v/>
       </c>
       <c r="L81" s="11">
@@ -8292,23 +8292,23 @@
         </is>
       </c>
       <c r="G82">
-        <f>'By Round'!G91</f>
+        <f>'By Round'!G90</f>
         <v/>
       </c>
       <c r="H82">
-        <f>'By Round'!H91</f>
+        <f>'By Round'!H90</f>
         <v/>
       </c>
       <c r="I82">
-        <f>'By Round'!I91</f>
+        <f>'By Round'!I90</f>
         <v/>
       </c>
       <c r="J82">
-        <f>'By Round'!J91</f>
+        <f>'By Round'!J90</f>
         <v/>
       </c>
       <c r="K82">
-        <f>'By Round'!K91</f>
+        <f>'By Round'!K90</f>
         <v/>
       </c>
       <c r="L82" s="11">
@@ -8844,23 +8844,23 @@
         </is>
       </c>
       <c r="G88">
-        <f>'By Round'!G11</f>
+        <f>'By Round'!G10</f>
         <v/>
       </c>
       <c r="H88">
-        <f>'By Round'!H11</f>
+        <f>'By Round'!H10</f>
         <v/>
       </c>
       <c r="I88">
-        <f>'By Round'!I11</f>
+        <f>'By Round'!I10</f>
         <v/>
       </c>
       <c r="J88">
-        <f>'By Round'!J11</f>
+        <f>'By Round'!J10</f>
         <v/>
       </c>
       <c r="K88">
-        <f>'By Round'!K11</f>
+        <f>'By Round'!K10</f>
         <v/>
       </c>
       <c r="L88" s="11">
@@ -8935,23 +8935,23 @@
         </is>
       </c>
       <c r="G89">
-        <f>'By Round'!G19</f>
+        <f>'By Round'!G18</f>
         <v/>
       </c>
       <c r="H89">
-        <f>'By Round'!H19</f>
+        <f>'By Round'!H18</f>
         <v/>
       </c>
       <c r="I89">
-        <f>'By Round'!I19</f>
+        <f>'By Round'!I18</f>
         <v/>
       </c>
       <c r="J89">
-        <f>'By Round'!J19</f>
+        <f>'By Round'!J18</f>
         <v/>
       </c>
       <c r="K89">
-        <f>'By Round'!K19</f>
+        <f>'By Round'!K18</f>
         <v/>
       </c>
       <c r="L89" s="11">
@@ -9026,23 +9026,23 @@
         </is>
       </c>
       <c r="G90">
-        <f>'By Round'!G67</f>
+        <f>'By Round'!G66</f>
         <v/>
       </c>
       <c r="H90">
-        <f>'By Round'!H67</f>
+        <f>'By Round'!H66</f>
         <v/>
       </c>
       <c r="I90">
-        <f>'By Round'!I67</f>
+        <f>'By Round'!I66</f>
         <v/>
       </c>
       <c r="J90">
-        <f>'By Round'!J67</f>
+        <f>'By Round'!J66</f>
         <v/>
       </c>
       <c r="K90">
-        <f>'By Round'!K67</f>
+        <f>'By Round'!K66</f>
         <v/>
       </c>
       <c r="L90" s="11">
@@ -9117,23 +9117,23 @@
         </is>
       </c>
       <c r="G91">
-        <f>'By Round'!G75</f>
+        <f>'By Round'!G74</f>
         <v/>
       </c>
       <c r="H91">
-        <f>'By Round'!H75</f>
+        <f>'By Round'!H74</f>
         <v/>
       </c>
       <c r="I91">
-        <f>'By Round'!I75</f>
+        <f>'By Round'!I74</f>
         <v/>
       </c>
       <c r="J91">
-        <f>'By Round'!J75</f>
+        <f>'By Round'!J74</f>
         <v/>
       </c>
       <c r="K91">
-        <f>'By Round'!K75</f>
+        <f>'By Round'!K74</f>
         <v/>
       </c>
       <c r="L91" s="11">
@@ -9208,23 +9208,23 @@
         </is>
       </c>
       <c r="G92">
-        <f>'By Round'!G83</f>
+        <f>'By Round'!G82</f>
         <v/>
       </c>
       <c r="H92">
-        <f>'By Round'!H83</f>
+        <f>'By Round'!H82</f>
         <v/>
       </c>
       <c r="I92">
-        <f>'By Round'!I83</f>
+        <f>'By Round'!I82</f>
         <v/>
       </c>
       <c r="J92">
-        <f>'By Round'!J83</f>
+        <f>'By Round'!J82</f>
         <v/>
       </c>
       <c r="K92">
-        <f>'By Round'!K83</f>
+        <f>'By Round'!K82</f>
         <v/>
       </c>
       <c r="L92" s="11">
@@ -11423,6 +11423,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="C1" s="3" t="inlineStr">

</xml_diff>

<commit_message>
even number mitchell tables
</commit_message>
<xml_diff>
--- a/howell10.xlsx
+++ b/howell10.xlsx
@@ -511,7 +511,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>For public domain. No rights reserved. Generated on Feb 04, 2026.</t>
+          <t>For public domain. No rights reserved. Generated on Feb 05, 2026.</t>
         </is>
       </c>
     </row>
@@ -595,12 +595,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Name 58</t>
+          <t>Name 78</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Name 69</t>
+          <t>Name 27</t>
         </is>
       </c>
       <c r="D10" s="4">
@@ -618,12 +618,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Name 17</t>
+          <t>Name 85</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Name 39</t>
+          <t>Name 21</t>
         </is>
       </c>
       <c r="D11" s="4">
@@ -641,12 +641,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Name 53</t>
+          <t>Name 76</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Name 68</t>
+          <t>Name 50</t>
         </is>
       </c>
       <c r="D12" s="4">
@@ -664,12 +664,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Name 24</t>
+          <t>Name 88</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Name 33</t>
+          <t>Name 65</t>
         </is>
       </c>
       <c r="D13" s="4">
@@ -687,12 +687,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Name 64</t>
+          <t>Name 43</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Name 14</t>
+          <t>Name 74</t>
         </is>
       </c>
       <c r="D14" s="4">
@@ -710,12 +710,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Name 45</t>
+          <t>Name 69</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Name 32</t>
+          <t>Name 36</t>
         </is>
       </c>
       <c r="D15" s="4">
@@ -733,12 +733,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Name 23</t>
+          <t>Name 50</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Name 75</t>
+          <t>Name 40</t>
         </is>
       </c>
       <c r="D16" s="4">
@@ -756,12 +756,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Name 23</t>
+          <t>Name 83</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Name 55</t>
+          <t>Name 14</t>
         </is>
       </c>
       <c r="D17" s="4">
@@ -779,12 +779,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Name 87</t>
+          <t>Name 77</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Name 24</t>
+          <t>Name 53</t>
         </is>
       </c>
       <c r="D18" s="4">
@@ -802,12 +802,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Name 84</t>
+          <t>Name 54</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Name 42</t>
+          <t>Name 11</t>
         </is>
       </c>
       <c r="D19" s="4">

</xml_diff>

<commit_message>
result changed to made/down
</commit_message>
<xml_diff>
--- a/howell10.xlsx
+++ b/howell10.xlsx
@@ -511,7 +511,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>For public domain. No rights reserved. Generated on Feb 11, 2026.</t>
+          <t>For public domain. No rights reserved. Generated on Feb 12, 2026.</t>
         </is>
       </c>
     </row>
@@ -595,12 +595,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Name 40</t>
+          <t>Name 61</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Name 60</t>
+          <t>Name 55</t>
         </is>
       </c>
       <c r="D10" s="4">
@@ -618,12 +618,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Name 22</t>
+          <t>Name 75</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Name 76</t>
+          <t>Name 59</t>
         </is>
       </c>
       <c r="D11" s="4">
@@ -641,12 +641,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Name 54</t>
+          <t>Name 83</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Name 12</t>
+          <t>Name 83</t>
         </is>
       </c>
       <c r="D12" s="4">
@@ -664,12 +664,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Name 82</t>
+          <t>Name 34</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Name 57</t>
+          <t>Name 73</t>
         </is>
       </c>
       <c r="D13" s="4">
@@ -687,12 +687,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Name 89</t>
+          <t>Name 46</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Name 85</t>
+          <t>Name 27</t>
         </is>
       </c>
       <c r="D14" s="4">
@@ -710,12 +710,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Name 80</t>
+          <t>Name 13</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Name 63</t>
+          <t>Name 36</t>
         </is>
       </c>
       <c r="D15" s="4">
@@ -733,12 +733,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Name 62</t>
+          <t>Name 63</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Name 45</t>
+          <t>Name 52</t>
         </is>
       </c>
       <c r="D16" s="4">
@@ -756,12 +756,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Name 25</t>
+          <t>Name 69</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Name 50</t>
+          <t>Name 77</t>
         </is>
       </c>
       <c r="D17" s="4">
@@ -779,12 +779,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Name 53</t>
+          <t>Name 64</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Name 60</t>
+          <t>Name 21</t>
         </is>
       </c>
       <c r="D18" s="4">
@@ -802,12 +802,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Name 63</t>
+          <t>Name 33</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Name 44</t>
+          <t>Name 73</t>
         </is>
       </c>
       <c r="D19" s="4">

</xml_diff>